<commit_message>
update arduino source add debug mode, fix bug
</commit_message>
<xml_diff>
--- a/documents/excel/array data structure.xlsx
+++ b/documents/excel/array data structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester8\tugas akhir\project_skripsi\documents\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8BC4A-739B-4861-AC2D-87EDCCD60675}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B861E8-86E5-4657-8761-AAF1733D03E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{DF5A165D-80A9-4BD6-BA1E-BC231576B079}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="119">
   <si>
     <t>index</t>
   </si>
@@ -286,13 +286,109 @@
   </si>
   <si>
     <t>index 5 signify the current ph value floating number</t>
+  </si>
+  <si>
+    <t>Array Structure : debug</t>
+  </si>
+  <si>
+    <t>index 1 signify led channel red value from 0 - 255</t>
+  </si>
+  <si>
+    <t>signify led fan strength value</t>
+  </si>
+  <si>
+    <t>signify led value strength channel : red</t>
+  </si>
+  <si>
+    <t>signify led value strength channel : green</t>
+  </si>
+  <si>
+    <t>signify led value strength channel : blue</t>
+  </si>
+  <si>
+    <t>signify led value strength channel : white</t>
+  </si>
+  <si>
+    <t>contain led &amp; fan strength value</t>
+  </si>
+  <si>
+    <t>signify dosing pump liquid to discharge pump channel : alkalinity</t>
+  </si>
+  <si>
+    <t>signify dosing pump liquid to discharge pump channel : calcium</t>
+  </si>
+  <si>
+    <t>signify dosing pump liquid to discharge pump channel : magnesium</t>
+  </si>
+  <si>
+    <t>contain dosing pump needed liquid to discharge</t>
+  </si>
+  <si>
+    <t>index 6 signify dosing pump needed liquid to discharge in pump channel : alk</t>
+  </si>
+  <si>
+    <t>index 7 signify dosing pump needed liquid to discharge in pump channel : cal</t>
+  </si>
+  <si>
+    <t>index 8 signify dosing pump needed liquid to discharge in pump channel : mag</t>
+  </si>
+  <si>
+    <t>index 2 signify led channel green value from 0 - 255</t>
+  </si>
+  <si>
+    <t>index 3 signify led channel blue value from 0 - 255</t>
+  </si>
+  <si>
+    <t>index 4 signify led channel white value from 0 - 255</t>
+  </si>
+  <si>
+    <t>index 5 signify led fan strength value from 0 - 255</t>
+  </si>
+  <si>
+    <t>signify top up pump discharge activation status</t>
+  </si>
+  <si>
+    <t>signify return pump activation status</t>
+  </si>
+  <si>
+    <t>signify wavemaker : left activation status</t>
+  </si>
+  <si>
+    <t>signify wavemaker : right activation status</t>
+  </si>
+  <si>
+    <t>index 10 signify the activation status value for top up pump</t>
+  </si>
+  <si>
+    <t>index 11 signify the activation status value for return pump</t>
+  </si>
+  <si>
+    <t>index 12 signify the activation status value for left wavemaker pump</t>
+  </si>
+  <si>
+    <t>index 13 signify the activation status value for right wavemaker pump</t>
+  </si>
+  <si>
+    <t>contain top up pump activation value</t>
+  </si>
+  <si>
+    <t>contain return pump activation value</t>
+  </si>
+  <si>
+    <t>contain wavemaker : left pump activation value</t>
+  </si>
+  <si>
+    <t>contain wavemaker : right pump activation value</t>
+  </si>
+  <si>
+    <t>signify debug mode flag status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,6 +426,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -491,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -621,19 +723,31 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -645,20 +759,44 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -974,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9320DF6-BE0E-4B4E-8BC9-E381E4019864}">
-  <dimension ref="A3:I124"/>
+  <dimension ref="A3:I125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,14 +1130,14 @@
   <sheetData>
     <row r="3" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
     </row>
     <row r="5" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
@@ -1037,7 +1175,7 @@
       <c r="F6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="63" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="13" t="s">
@@ -1060,7 +1198,7 @@
       <c r="F7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="64"/>
       <c r="I7" s="20" t="s">
         <v>29</v>
       </c>
@@ -1081,7 +1219,7 @@
       <c r="F8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="55"/>
+      <c r="G8" s="64"/>
     </row>
     <row r="9" spans="2:9" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
@@ -1099,7 +1237,7 @@
       <c r="F9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="54"/>
+      <c r="G9" s="65"/>
     </row>
     <row r="10" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
@@ -1117,7 +1255,7 @@
       <c r="F10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="45" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1137,7 +1275,7 @@
       <c r="F11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="56" t="s">
+      <c r="G11" s="45" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1219,14 +1357,14 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="2:9" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
-      <c r="G21" s="52"/>
+      <c r="C21" s="55"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" spans="2:9" ht="18" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
@@ -1264,7 +1402,7 @@
       <c r="F23" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="47" t="s">
+      <c r="G23" s="60" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1284,7 +1422,7 @@
       <c r="F24" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="47"/>
+      <c r="G24" s="60"/>
     </row>
     <row r="25" spans="2:9" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
@@ -1302,7 +1440,7 @@
       <c r="F25" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="47"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="2:9" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B26" s="12">
@@ -1320,7 +1458,7 @@
       <c r="F26" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="47"/>
+      <c r="G26" s="60"/>
     </row>
     <row r="27" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="12">
@@ -1338,7 +1476,7 @@
       <c r="F27" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="47" t="s">
+      <c r="G27" s="60" t="s">
         <v>76</v>
       </c>
       <c r="I27" s="13" t="s">
@@ -1361,7 +1499,7 @@
       <c r="F28" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="47"/>
+      <c r="G28" s="60"/>
       <c r="I28" s="35" t="s">
         <v>60</v>
       </c>
@@ -1382,7 +1520,7 @@
       <c r="F29" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="47"/>
+      <c r="G29" s="60"/>
       <c r="I29" s="34" t="s">
         <v>61</v>
       </c>
@@ -1403,7 +1541,7 @@
       <c r="F30" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="47"/>
+      <c r="G30" s="60"/>
       <c r="I30" s="41" t="s">
         <v>74</v>
       </c>
@@ -1424,7 +1562,7 @@
       <c r="F31" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="47" t="s">
+      <c r="G31" s="60" t="s">
         <v>75</v>
       </c>
       <c r="I31" s="40" t="s">
@@ -1447,7 +1585,7 @@
       <c r="F32" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="47"/>
+      <c r="G32" s="60"/>
     </row>
     <row r="33" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B33" s="12">
@@ -1465,7 +1603,7 @@
       <c r="F33" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="47"/>
+      <c r="G33" s="60"/>
     </row>
     <row r="34" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B34" s="12">
@@ -1483,7 +1621,7 @@
       <c r="F34" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="47"/>
+      <c r="G34" s="60"/>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="12">
@@ -1501,7 +1639,7 @@
       <c r="F35" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="47" t="s">
+      <c r="G35" s="60" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1521,7 +1659,7 @@
       <c r="F36" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="47"/>
+      <c r="G36" s="60"/>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="12">
@@ -1539,7 +1677,7 @@
       <c r="F37" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="47"/>
+      <c r="G37" s="60"/>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="12">
@@ -1562,10 +1700,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="48">
+      <c r="B39" s="67">
         <v>16</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="67" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="42">
@@ -1577,13 +1715,13 @@
       <c r="F39" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="49" t="s">
+      <c r="G39" s="61" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="67"/>
       <c r="D40" s="42">
         <v>2</v>
       </c>
@@ -1593,11 +1731,11 @@
       <c r="F40" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="49"/>
+      <c r="G40" s="61"/>
     </row>
     <row r="41" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="67"/>
       <c r="D41" s="42">
         <v>3</v>
       </c>
@@ -1607,13 +1745,13 @@
       <c r="F41" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G41" s="49"/>
+      <c r="G41" s="61"/>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="45">
+      <c r="B42" s="66">
         <v>17</v>
       </c>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="66" t="s">
         <v>68</v>
       </c>
       <c r="D42" s="44">
@@ -1625,13 +1763,13 @@
       <c r="F42" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="46" t="s">
+      <c r="G42" s="62" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="45"/>
-      <c r="C43" s="45"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
       <c r="D43" s="44">
         <v>2</v>
       </c>
@@ -1641,11 +1779,11 @@
       <c r="F43" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="46"/>
+      <c r="G43" s="62"/>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="45"/>
-      <c r="C44" s="45"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="44">
         <v>3</v>
       </c>
@@ -1655,7 +1793,7 @@
       <c r="F44" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="G44" s="46"/>
+      <c r="G44" s="62"/>
     </row>
     <row r="45" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
@@ -1663,7 +1801,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="57"/>
+      <c r="G45" s="46"/>
     </row>
     <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
@@ -1671,7 +1809,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="57"/>
+      <c r="G46" s="46"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
@@ -1698,213 +1836,354 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+    <row r="50" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="56"/>
+    </row>
+    <row r="51" spans="2:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="B51" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="12">
+        <v>0</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="F52" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" s="57" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="12">
+        <v>1</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="58"/>
+    </row>
+    <row r="54" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="12">
+        <v>2</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="F54" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54" s="58"/>
+    </row>
+    <row r="55" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="12">
+        <v>3</v>
+      </c>
+      <c r="C55" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="F55" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55" s="58"/>
+    </row>
+    <row r="56" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="12">
+        <v>4</v>
+      </c>
+      <c r="C56" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="F56" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" s="59"/>
+    </row>
+    <row r="57" spans="2:7" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="12">
+        <v>5</v>
+      </c>
+      <c r="C57" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G57" s="57" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="12">
+        <v>6</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G58" s="58"/>
+    </row>
+    <row r="59" spans="2:7" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="12">
+        <v>7</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F59" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G59" s="59"/>
+    </row>
+    <row r="60" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="12">
+        <v>8</v>
+      </c>
+      <c r="C60" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G60" s="47" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="12">
+        <v>9</v>
+      </c>
+      <c r="C61" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="F61" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G61" s="47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="12">
+        <v>10</v>
+      </c>
+      <c r="C62" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G62" s="47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B63" s="12">
+        <v>11</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="F63" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G63" s="47" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="B64" s="68">
+        <v>12</v>
+      </c>
+      <c r="C64" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" s="69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="49"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="49"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="51"/>
+      <c r="G66" s="52"/>
+    </row>
+    <row r="67" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="49"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="49"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="51"/>
+      <c r="G67" s="52"/>
+    </row>
+    <row r="68" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="49"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="51"/>
+      <c r="G68" s="53"/>
+    </row>
+    <row r="69" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="48"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="48"/>
+    </row>
+    <row r="70" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="48"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
+      <c r="F70" s="48"/>
+      <c r="G70" s="48"/>
+    </row>
+    <row r="71" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="48"/>
+      <c r="C71" s="48"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
+      <c r="F71" s="48"/>
+      <c r="G71" s="48"/>
+    </row>
+    <row r="72" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="48"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
+    </row>
+    <row r="73" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="48"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+    </row>
+    <row r="74" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="48"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="48"/>
     </row>
     <row r="75" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
     </row>
     <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="1"/>
@@ -2283,26 +2562,37 @@
       <c r="G122" s="1"/>
     </row>
     <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="1"/>
       <c r="G123" s="1"/>
     </row>
     <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G124" s="1"/>
     </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G125" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="G35:G37"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="G42:G44"/>
+  <mergeCells count="16">
+    <mergeCell ref="G31:G34"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="G23:G26"/>
     <mergeCell ref="G6:G9"/>
     <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G31:G34"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="B50:G50"/>
+    <mergeCell ref="G52:G56"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="G35:G37"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="G42:G44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update on new method of crud
</commit_message>
<xml_diff>
--- a/documents/excel/array data structure.xlsx
+++ b/documents/excel/array data structure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kuliah\semester8\tugas akhir\project_skripsi\documents\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAFCB69-1DAA-4299-B7A7-0DFD4564330E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F016DF-1BDD-415B-97E5-697C7C9D08E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{DF5A165D-80A9-4BD6-BA1E-BC231576B079}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="164">
   <si>
     <t>index</t>
   </si>
@@ -414,18 +414,6 @@
     <t>Arduino (master)</t>
   </si>
   <si>
-    <t>Esp8266(slave)</t>
-  </si>
-  <si>
-    <t>ping esp when waifi status is true and instruct esp to ping on firebase for any new data.</t>
-  </si>
-  <si>
-    <t>ping esp when wifi status is false.</t>
-  </si>
-  <si>
-    <t>ping esp when arduino want to send array of sensor data to be uploaded to firebase.</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -456,12 +444,6 @@
     <t>l</t>
   </si>
   <si>
-    <t>ping arduino master that new debug device data is present and succesfully fetched ready to be transmitted through serial communication</t>
-  </si>
-  <si>
-    <t>ping arduino master that new device data is present and succesfully fetched ready to be transmitted through serial communication</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -480,24 +462,6 @@
     <t>r</t>
   </si>
   <si>
-    <t>response for arduino master 'a' or 'c' ping that wifi and firebase is still offline</t>
-  </si>
-  <si>
-    <t>response for arduino master 'a' or 'c' ping that wifi is online but firebase is still offline</t>
-  </si>
-  <si>
-    <t>response for arduino master 'a' or 'c' ping that wifi and firebase is already online</t>
-  </si>
-  <si>
-    <t>Arduino (slave)</t>
-  </si>
-  <si>
-    <t>Arduino(slave)</t>
-  </si>
-  <si>
-    <t>ping arduino slave for latest sensor readings</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
@@ -507,20 +471,988 @@
     <t>N/A</t>
   </si>
   <si>
-    <t xml:space="preserve">response for arduino master 'd' ping and preparing to temp sensor reading data </t>
-  </si>
-  <si>
-    <t xml:space="preserve">response for arduino master 'd' ping and preparing to ph sensor reading data </t>
-  </si>
-  <si>
-    <t xml:space="preserve">response for arduino master 'd' ping and preparing to send waterlevel reading data </t>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">network_endpoint_esp8266 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sensor_side_arduino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">when </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> want to send array of wifi auth data to be used as new wifi point by  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and it will instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to halt any communication attempt. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> when </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> done sending array of wifi auth data to be used as new wifi point by  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and it will instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to continue any communication attempt. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arduino (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esp8266(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arduino (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that new device data is present and succesfully fetched ready to be transmitted through serial communication to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sensor_side_arduino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>to halt any communication attempt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sensor_side_arduino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">that new debug data is present and succesfully fetched ready to be transmitted through serial communication to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to halt any communication attempt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arduino (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">sensor_side_arduino </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">that new debug data is succesfully transmitted through serial communication to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, and instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to continue any communication attempt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that new sensor data array is ready to be transmitted through serial communication to  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">network_endpoint_esp8266 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">and to be uploaded to firebase, and instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to halt any communication attempt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Arduino (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) and Esp8266(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ping </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that new sensor data array is done transmitted through serial communication to  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">network_endpoint_esp8266 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">and to be uploaded to firebase, and instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to continue any communication attempt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Esp8266(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>network_endpoint_esp8266</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) and Arduino (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>master_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>broadcast to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> any arduino device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that indicates wifi and firebase is still offline to instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to halt any communication attempt until the network is restored.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">broadcast to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>any arduino device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that indicates wifi is online but firebase is still offline to instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to halt any communication attempt until the network is restored.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">broadcast to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>any arduino device</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> that indicates wifi and firebase is already online to instruct </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>sensor_side_arduino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to continue any communication attempt.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -580,6 +1512,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -917,6 +1857,9 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -960,9 +1903,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1281,8 +2221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9320DF6-BE0E-4B4E-8BC9-E381E4019864}">
   <dimension ref="A3:O125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="H11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,28 +2235,28 @@
     <col min="9" max="9" width="27.28515625" customWidth="1"/>
     <col min="11" max="11" width="5.28515625" customWidth="1"/>
     <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.7109375" customWidth="1"/>
+    <col min="13" max="13" width="54.7109375" customWidth="1"/>
+    <col min="14" max="14" width="89.28515625" customWidth="1"/>
     <col min="15" max="15" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="62"/>
-      <c r="K4" s="58" t="s">
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="63"/>
+      <c r="K4" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
     </row>
     <row r="5" spans="2:15" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
@@ -1353,7 +2293,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="9">
         <v>0</v>
       </c>
@@ -1369,7 +2309,7 @@
       <c r="F6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="69" t="s">
+      <c r="G6" s="70" t="s">
         <v>20</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -1382,16 +2322,16 @@
         <v>125</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="O6" s="53" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="54" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>1</v>
       </c>
@@ -1407,7 +2347,7 @@
       <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="70"/>
+      <c r="G7" s="71"/>
       <c r="I7" s="19" t="s">
         <v>29</v>
       </c>
@@ -1418,13 +2358,13 @@
         <v>126</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="O7" s="53" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
@@ -1443,7 +2383,7 @@
       <c r="F8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="70"/>
+      <c r="G8" s="71"/>
       <c r="K8" s="9">
         <v>3</v>
       </c>
@@ -1451,10 +2391,10 @@
         <v>127</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>129</v>
+        <v>147</v>
       </c>
       <c r="O8" s="53" t="s">
         <v>130</v>
@@ -1476,21 +2416,21 @@
       <c r="F9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="71"/>
+      <c r="G9" s="72"/>
       <c r="K9" s="9">
         <v>4</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="O9" s="53" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1516,16 +2456,16 @@
         <v>5</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="O10" s="53" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
@@ -1551,19 +2491,19 @@
         <v>6</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="N11" s="9" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="O11" s="53" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="9">
         <v>6</v>
       </c>
@@ -1586,19 +2526,19 @@
         <v>7</v>
       </c>
       <c r="L12" s="54" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="M12" s="54" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="N12" s="54" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="O12" s="29" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="31.5" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="75.75" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>7</v>
       </c>
@@ -1621,53 +2561,53 @@
         <v>8</v>
       </c>
       <c r="L13" s="54" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="N13" s="54" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="O13" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K14" s="54">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" s="1" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="8">
         <v>9</v>
       </c>
-      <c r="L14" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="M14" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="N14" s="54" t="s">
-        <v>128</v>
+      <c r="L14" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="O14" s="29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="45" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="105" x14ac:dyDescent="0.25">
       <c r="K15" s="54">
         <v>10</v>
       </c>
       <c r="L15" s="54" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="M15" s="54" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="N15" s="54" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="O15" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="20"/>
       <c r="C16" s="21"/>
       <c r="D16" s="56"/>
@@ -1678,19 +2618,19 @@
         <v>11</v>
       </c>
       <c r="L16" s="54" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="M16" s="54" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="N16" s="54" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="O16" s="29" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" ht="90" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="56"/>
@@ -1701,19 +2641,19 @@
         <v>12</v>
       </c>
       <c r="L17" s="54" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="M17" s="54" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="N17" s="54" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
       <c r="O17" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="120" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -1724,19 +2664,19 @@
         <v>13</v>
       </c>
       <c r="L18" s="55" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="M18" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N18" s="55" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="O18" s="26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" ht="120" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1746,19 +2686,19 @@
         <v>14</v>
       </c>
       <c r="L19" s="55" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="M19" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N19" s="55" t="s">
-        <v>128</v>
+        <v>158</v>
       </c>
       <c r="O19" s="26" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1768,41 +2708,41 @@
         <v>15</v>
       </c>
       <c r="L20" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="N20" s="55" t="s">
         <v>147</v>
       </c>
-      <c r="M20" s="55" t="s">
-        <v>154</v>
-      </c>
-      <c r="N20" s="55" t="s">
-        <v>128</v>
-      </c>
       <c r="O20" s="26" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="60" t="s">
+      <c r="B21" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="61"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="63"/>
       <c r="K21" s="55">
         <v>16</v>
       </c>
       <c r="L21" s="55" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="M21" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N21" s="55" t="s">
         <v>128</v>
       </c>
       <c r="O21" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="2:15" ht="18" x14ac:dyDescent="0.25">
@@ -1828,16 +2768,16 @@
         <v>17</v>
       </c>
       <c r="L22" s="55" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="M22" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N22" s="55" t="s">
         <v>128</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
@@ -1856,23 +2796,23 @@
       <c r="F23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G23" s="66" t="s">
+      <c r="G23" s="67" t="s">
         <v>40</v>
       </c>
       <c r="K23" s="55">
         <v>18</v>
       </c>
       <c r="L23" s="55" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="M23" s="55" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N23" s="55" t="s">
         <v>128</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
@@ -1891,12 +2831,12 @@
       <c r="F24" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="66"/>
+      <c r="G24" s="67"/>
       <c r="K24" s="5">
         <v>19</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
@@ -1915,12 +2855,12 @@
       <c r="F25" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G25" s="66"/>
+      <c r="G25" s="67"/>
       <c r="K25" s="5">
         <v>20</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="45.75" x14ac:dyDescent="0.25">
@@ -1939,7 +2879,7 @@
       <c r="F26" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="66"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
@@ -1957,7 +2897,7 @@
       <c r="F27" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="66" t="s">
+      <c r="G27" s="67" t="s">
         <v>76</v>
       </c>
       <c r="I27" s="12" t="s">
@@ -1980,7 +2920,7 @@
       <c r="F28" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G28" s="66"/>
+      <c r="G28" s="67"/>
       <c r="I28" s="31" t="s">
         <v>60</v>
       </c>
@@ -2001,7 +2941,7 @@
       <c r="F29" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="66"/>
+      <c r="G29" s="67"/>
       <c r="I29" s="30" t="s">
         <v>61</v>
       </c>
@@ -2022,7 +2962,7 @@
       <c r="F30" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="66"/>
+      <c r="G30" s="67"/>
       <c r="I30" s="37" t="s">
         <v>74</v>
       </c>
@@ -2043,7 +2983,7 @@
       <c r="F31" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="66" t="s">
+      <c r="G31" s="67" t="s">
         <v>75</v>
       </c>
       <c r="I31" s="36" t="s">
@@ -2066,7 +3006,7 @@
       <c r="F32" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G32" s="66"/>
+      <c r="G32" s="67"/>
     </row>
     <row r="33" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
@@ -2084,7 +3024,7 @@
       <c r="F33" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="66"/>
+      <c r="G33" s="67"/>
     </row>
     <row r="34" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
@@ -2102,7 +3042,7 @@
       <c r="F34" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="66"/>
+      <c r="G34" s="67"/>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
@@ -2120,7 +3060,7 @@
       <c r="F35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="66" t="s">
+      <c r="G35" s="67" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2140,7 +3080,7 @@
       <c r="F36" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G36" s="66"/>
+      <c r="G36" s="67"/>
     </row>
     <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
@@ -2158,7 +3098,7 @@
       <c r="F37" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G37" s="66"/>
+      <c r="G37" s="67"/>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
@@ -2181,10 +3121,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="73">
+      <c r="B39" s="58">
         <v>16</v>
       </c>
-      <c r="C39" s="73" t="s">
+      <c r="C39" s="58" t="s">
         <v>62</v>
       </c>
       <c r="D39" s="38">
@@ -2196,13 +3136,13 @@
       <c r="F39" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="G39" s="67" t="s">
+      <c r="G39" s="68" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="73"/>
-      <c r="C40" s="73"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="58"/>
       <c r="D40" s="38">
         <v>2</v>
       </c>
@@ -2212,11 +3152,11 @@
       <c r="F40" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="G40" s="67"/>
+      <c r="G40" s="68"/>
     </row>
     <row r="41" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="58"/>
       <c r="D41" s="38">
         <v>3</v>
       </c>
@@ -2226,13 +3166,13 @@
       <c r="F41" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="G41" s="67"/>
+      <c r="G41" s="68"/>
     </row>
     <row r="42" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B42" s="72">
+      <c r="B42" s="73">
         <v>17</v>
       </c>
-      <c r="C42" s="72" t="s">
+      <c r="C42" s="73" t="s">
         <v>68</v>
       </c>
       <c r="D42" s="40">
@@ -2244,13 +3184,13 @@
       <c r="F42" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G42" s="68" t="s">
+      <c r="G42" s="69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
       <c r="D43" s="40">
         <v>2</v>
       </c>
@@ -2260,11 +3200,11 @@
       <c r="F43" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="68"/>
+      <c r="G43" s="69"/>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="72"/>
-      <c r="C44" s="72"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
       <c r="D44" s="40">
         <v>3</v>
       </c>
@@ -2274,7 +3214,7 @@
       <c r="F44" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="G44" s="68"/>
+      <c r="G44" s="69"/>
     </row>
     <row r="45" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
@@ -2318,14 +3258,14 @@
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="2:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="60" t="s">
+      <c r="B50" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="61"/>
-      <c r="D50" s="61"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="62"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="62"/>
+      <c r="G50" s="63"/>
     </row>
     <row r="51" spans="2:7" ht="18" x14ac:dyDescent="0.25">
       <c r="B51" s="22" t="s">
@@ -2363,7 +3303,7 @@
       <c r="F52" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G52" s="63" t="s">
+      <c r="G52" s="64" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2383,7 +3323,7 @@
       <c r="F53" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G53" s="64"/>
+      <c r="G53" s="65"/>
     </row>
     <row r="54" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B54" s="11">
@@ -2401,7 +3341,7 @@
       <c r="F54" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G54" s="64"/>
+      <c r="G54" s="65"/>
     </row>
     <row r="55" spans="2:7" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B55" s="11">
@@ -2419,7 +3359,7 @@
       <c r="F55" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G55" s="64"/>
+      <c r="G55" s="65"/>
     </row>
     <row r="56" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="11">
@@ -2437,7 +3377,7 @@
       <c r="F56" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G56" s="65"/>
+      <c r="G56" s="66"/>
     </row>
     <row r="57" spans="2:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B57" s="11">
@@ -2455,7 +3395,7 @@
       <c r="F57" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G57" s="63" t="s">
+      <c r="G57" s="64" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2475,7 +3415,7 @@
       <c r="F58" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G58" s="64"/>
+      <c r="G58" s="65"/>
     </row>
     <row r="59" spans="2:7" ht="45.75" x14ac:dyDescent="0.25">
       <c r="B59" s="11">
@@ -2493,7 +3433,7 @@
       <c r="F59" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="G59" s="65"/>
+      <c r="G59" s="66"/>
     </row>
     <row r="60" spans="2:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="11">
@@ -3058,6 +3998,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B39:B41"/>
     <mergeCell ref="C39:C41"/>
     <mergeCell ref="K4:O4"/>
     <mergeCell ref="B50:G50"/>
@@ -3074,7 +4015,6 @@
     <mergeCell ref="G31:G34"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B39:B41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>